<commit_message>
Added Day-12 project file
</commit_message>
<xml_diff>
--- a/Twitter_schema.xlsx
+++ b/Twitter_schema.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" tabRatio="734" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" tabRatio="734"/>
   </bookViews>
   <sheets>
     <sheet name="requirements" sheetId="3" r:id="rId1"/>
     <sheet name="User_tbl" sheetId="1" r:id="rId2"/>
     <sheet name="user_profile_tbl" sheetId="12" r:id="rId3"/>
-    <sheet name="Tweeter_tbl" sheetId="2" r:id="rId4"/>
+    <sheet name="Tweet_tbl" sheetId="2" r:id="rId4"/>
     <sheet name="follower_tbl" sheetId="4" r:id="rId5"/>
     <sheet name="Comment_tbl" sheetId="5" r:id="rId6"/>
     <sheet name="Like_tweet_tbl" sheetId="9" r:id="rId7"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="139">
   <si>
     <t>User Table</t>
   </si>
@@ -65,9 +65,6 @@
     <t>created_on</t>
   </si>
   <si>
-    <t>Tweeter Table</t>
-  </si>
-  <si>
     <t>user_id</t>
   </si>
   <si>
@@ -227,9 +224,6 @@
     <t>modified_on</t>
   </si>
   <si>
-    <t>creation_time</t>
-  </si>
-  <si>
     <t>Phase</t>
   </si>
   <si>
@@ -447,13 +441,22 @@
   </si>
   <si>
     <t>completed</t>
+  </si>
+  <si>
+    <t>Tweet Table</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>Edit the tweet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,6 +522,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -541,7 +558,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -564,6 +581,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
@@ -576,13 +595,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -871,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -886,203 +905,219 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C1" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="C1" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="J2" s="2" t="s">
-        <v>136</v>
+      <c r="J2" s="12" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="14">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>71</v>
+      <c r="B3" s="14" t="s">
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" s="16"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="14"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="14"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="14"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="2" t="s">
-        <v>67</v>
+        <v>121</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="J7" s="2" t="s">
+      <c r="B7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="16">
+        <v>2</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="1"/>
-      <c r="B8" s="11"/>
-    </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" s="14">
-        <v>2</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>5</v>
-      </c>
+      <c r="A9" s="16"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="16"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="14"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="2" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="16"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" s="14"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="2" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="16"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" s="14"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13" s="14"/>
-      <c r="B13" s="12"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="12" t="s">
-        <v>79</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="14" t="s">
+        <v>77</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B18" s="12"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B18" s="14"/>
       <c r="C18" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B19" s="14"/>
+      <c r="C19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B19" s="12"/>
-      <c r="C19" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B20" s="12"/>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B20" s="14"/>
       <c r="C20" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B21" s="14"/>
       <c r="C21" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C33" s="8" t="s">
-        <v>73</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="C22" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C34" s="2" t="s">
-        <v>74</v>
+      <c r="C34" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C35" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C36" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C37" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C38" s="2" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C39" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C40" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B17:B21"/>
     <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B3:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1098,12 +1133,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1111,10 +1146,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1142,25 +1177,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>39</v>
-      </c>
       <c r="D2" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.5">
@@ -1171,19 +1206,19 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -1192,31 +1227,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1224,46 +1259,46 @@
         <v>6</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="I8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="N8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2"/>
     </row>
@@ -1275,46 +1310,46 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:15" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H12" s="2"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.5">
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.5">
       <c r="H26" s="3"/>
@@ -1353,55 +1388,55 @@
   <sheetData>
     <row r="1" spans="1:7" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+        <v>122</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1409,14 +1444,14 @@
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E5" s="4"/>
     </row>
@@ -1433,20 +1468,20 @@
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E7" s="4"/>
       <c r="G7" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1462,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -1478,12 +1513,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="A1" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C2" s="6"/>
@@ -1491,82 +1526,82 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="C3" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -1575,10 +1610,10 @@
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1607,66 +1642,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="A1" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="9"/>
       <c r="F2" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
@@ -1677,15 +1712,15 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1701,7 +1736,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -1713,54 +1748,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="A1" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -1768,16 +1803,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -1788,21 +1823,21 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1831,64 +1866,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="A1" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -1899,7 +1934,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1925,56 +1960,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="A1" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -2003,28 +2038,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="A1" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2032,13 +2067,13 @@
     </row>
     <row r="3" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -2047,16 +2082,16 @@
     </row>
     <row r="4" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -2064,16 +2099,16 @@
     </row>
     <row r="5" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>

</xml_diff>

<commit_message>
Added-day 14 files for twitter project
</commit_message>
<xml_diff>
--- a/Twitter_schema.xlsx
+++ b/Twitter_schema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" tabRatio="734"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" tabRatio="734" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="requirements" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="154">
   <si>
     <t>User Table</t>
   </si>
@@ -104,12 +104,6 @@
     <t>post a tweet</t>
   </si>
   <si>
-    <t>view tweets of others as well as his own</t>
-  </si>
-  <si>
-    <t>like the tweet</t>
-  </si>
-  <si>
     <t>delete the tweet</t>
   </si>
   <si>
@@ -284,9 +278,6 @@
     <t>FK-User table</t>
   </si>
   <si>
-    <t>Modified on</t>
-  </si>
-  <si>
     <t>Comment edit datetime</t>
   </si>
   <si>
@@ -480,6 +471,30 @@
   </si>
   <si>
     <t>Accept / Reject the follow Request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">view tweets of others </t>
+  </si>
+  <si>
+    <t>like /Unlike the tweet</t>
+  </si>
+  <si>
+    <t>modified on</t>
+  </si>
+  <si>
+    <t>Edit the comment</t>
+  </si>
+  <si>
+    <t>Delete the comment</t>
+  </si>
+  <si>
+    <t>can view comments,who commented,when</t>
+  </si>
+  <si>
+    <t>FK-&gt;Tweet_tbl</t>
+  </si>
+  <si>
+    <t>comment is on this tweet</t>
   </si>
 </sst>
 </file>
@@ -616,7 +631,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -643,6 +658,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
@@ -958,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -973,76 +991,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C1" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="C1" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="J2" s="12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="18">
+      <c r="A3" s="19">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>69</v>
+      <c r="B3" s="17" t="s">
+        <v>67</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="18"/>
-      <c r="B4" s="16"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="18"/>
-      <c r="B5" s="16"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
-      <c r="B6" s="16"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
@@ -1051,215 +1069,251 @@
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="18">
+      <c r="A8" s="19">
         <v>2</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" s="18"/>
-      <c r="B9" s="20"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="18"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="19"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="19"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="14"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" s="18"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="14"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" s="18"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="J12" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13" s="18"/>
-      <c r="B13" s="20"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" s="18"/>
-      <c r="B14" s="20"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" s="19"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="J14" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" s="18"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="J15" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A16" s="18"/>
-      <c r="B16" s="20"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C17" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.45">
       <c r="J18" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.45">
       <c r="J19" s="14"/>
     </row>
     <row r="20" spans="2:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="16" t="s">
-        <v>77</v>
+      <c r="B20" s="17" t="s">
+        <v>75</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J20" s="14"/>
+        <v>74</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="21" spans="2:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="16"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="16"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B23" s="16"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J23" s="14"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B24" s="16"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J24" s="14"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B25" s="16"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B26" s="16"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B27" s="16"/>
       <c r="C27" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C35" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C36" s="2" t="s">
-        <v>138</v>
+        <v>151</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B28" s="16"/>
+      <c r="C28" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B29" s="16"/>
+      <c r="C29" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="C30" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C38" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C39" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C40" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C41" s="2" t="s">
-        <v>73</v>
+      <c r="C39" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C42" s="2" t="s">
-        <v>75</v>
+      <c r="C42" s="8" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C43" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C44" s="2" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C45" s="2" t="s">
-        <v>117</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C46" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C47" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C48" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1288,12 +1342,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1301,10 +1355,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1332,25 +1386,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="19"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>38</v>
-      </c>
       <c r="D2" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.5">
@@ -1361,19 +1415,19 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -1382,31 +1436,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1425,10 +1479,10 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1447,13 +1501,13 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2"/>
     </row>
@@ -1465,46 +1519,46 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D10" s="2"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:15" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H12" s="2"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.5">
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.5">
       <c r="H26" s="3"/>
@@ -1542,40 +1596,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="A1" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1588,10 +1642,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1599,14 +1653,14 @@
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E5" s="4"/>
     </row>
@@ -1623,20 +1677,20 @@
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E7" s="4"/>
       <c r="G7" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1653,7 +1707,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -1668,12 +1722,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="A1" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C2" s="6"/>
@@ -1681,27 +1735,27 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -1720,10 +1774,10 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
@@ -1734,29 +1788,29 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -1766,7 +1820,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>4</v>
@@ -1786,7 +1840,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -1797,58 +1851,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A1" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="A1" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="D2" s="9"/>
       <c r="F2" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
@@ -1859,27 +1913,27 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
@@ -1890,15 +1944,15 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1914,7 +1968,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -1926,54 +1980,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="A1" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -1984,13 +2038,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -2001,21 +2055,21 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
-        <v>83</v>
+        <v>148</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2031,7 +2085,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -2044,50 +2098,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="A1" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -2095,13 +2149,13 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -2112,7 +2166,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2138,34 +2192,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="A1" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -2174,7 +2228,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2187,7 +2241,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -2201,10 +2255,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2216,28 +2270,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="A1" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2245,13 +2299,13 @@
     </row>
     <row r="3" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -2260,16 +2314,16 @@
     </row>
     <row r="4" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -2280,17 +2334,31 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>153</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>